<commit_message>
añadido manager BT. Bugfix
</commit_message>
<xml_diff>
--- a/sensors/social/sensorSocial.xlsx
+++ b/sensors/social/sensorSocial.xlsx
@@ -5,287 +5,292 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="533" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CUESTIONARIO" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="ANÁLISIS" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="90">
   <si>
-    <t>Marque con una X la opción elegida para cada una de las preguntas:</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Nunca</t>
-  </si>
-  <si>
-    <t>Rara vez</t>
-  </si>
-  <si>
-    <t>A veces</t>
-  </si>
-  <si>
-    <t>Normalmente</t>
-  </si>
-  <si>
-    <t>Siempre</t>
-  </si>
-  <si>
-    <t>Los empleados entregan las tareas a tiempo.</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>El personal hace un buen trabajo.</t>
-  </si>
-  <si>
-    <t>Los empleados muestran conductas apáticas o desinterés.</t>
-  </si>
-  <si>
-    <t>El personal llega tarde al trabajo.</t>
-  </si>
-  <si>
-    <t>Se convocan huelgas y paros en la organización.</t>
-  </si>
-  <si>
-    <t>Los empleados faltan al trabajo sin una causa justificada.</t>
-  </si>
-  <si>
-    <t>Los empleados afrontan las situaciones críticas como unidad.</t>
-  </si>
-  <si>
-    <t>Los empleados se esfuerzan por integrar a los nuevos miembros en la plantilla.</t>
-  </si>
-  <si>
-    <t>Los diferentes grupos de trabajo existentes colaboran entre sí.</t>
-  </si>
-  <si>
-    <t>La gente crea problemas hablando de otros a sus espaldas.</t>
-  </si>
-  <si>
-    <t>La diferencia de opiniones en el equipo de trabajo provoca enfados y/o discusiones.</t>
-  </si>
-  <si>
-    <t>El ambiente de trabajo es tenso por la mala relación entre algunos empleados.</t>
-  </si>
-  <si>
-    <t>Los jefes reconocen el trabajo bien hecho, y felicitan a los empleados por ello.</t>
-  </si>
-  <si>
-    <t>Los jefes dialogan con sus empleados sobre lo qué hacen bien en su trabajo y los aspectos que pueden mejorar.</t>
-  </si>
-  <si>
-    <t>Los empleados comentan los temas que les preocupan con sus superiores.</t>
-  </si>
-  <si>
-    <t>Los jefes valoran la opinión de los empleados.</t>
-  </si>
-  <si>
-    <t>Los jefes utilizan un tono autoritario para dirigirse a sus empleados.</t>
-  </si>
-  <si>
-    <t>Los jefes tratan de igual forma a todos los empleados.</t>
-  </si>
-  <si>
-    <t>Los empleados pueden tomar sus propias decisiones y utilizar su propia iniciativa para hacer su trabajo.</t>
-  </si>
-  <si>
-    <t>Los jefes se reúnen con los empleados para tomar decisiones sobre proyectos futuros.</t>
-  </si>
-  <si>
-    <t>Las responsabilidades importantes se concentran en una sola persona.</t>
-  </si>
-  <si>
-    <t>Se valoran  los nuevos enfoques e ideas en la realización de los trabajos.</t>
-  </si>
-  <si>
-    <t>Los trabajos son monótonos y repetitivos.</t>
-  </si>
-  <si>
-    <t>Los empleados cuentan con programas de formación para actualizar sus conocimientos.</t>
-  </si>
-  <si>
-    <t>Las tareas se asignan con tiempo suficiente para que se puedan realizar con calma.</t>
-  </si>
-  <si>
-    <t>Los empleados tienen oportunidades para hacer pequeños descansos a lo largo del día.</t>
-  </si>
-  <si>
-    <t>Los empleados tienen mucha carga de trabajo.</t>
-  </si>
-  <si>
-    <t>Se tienen en consideración las necesidades personales de los empleados a la hora de fijar sus horarios.</t>
-  </si>
-  <si>
-    <t>Los horarios permiten la conciliación de la vida familiar y personal con la vida laboral.</t>
-  </si>
-  <si>
-    <t>Ante una necesidad personal o familiar extraordinaria, se busca la mejor solución.</t>
-  </si>
-  <si>
-    <t>Los empleados tienen dudas sobre cómo realizar sus tareas.</t>
-  </si>
-  <si>
-    <t>Se informa a los empleados de cómo contribuye su trabajo a la organización.</t>
-  </si>
-  <si>
-    <t>Los jefes estimulan a los empleados para que sean precisos y ordenados.</t>
-  </si>
-  <si>
-    <t>Se informa a los empleados de la situación y resultados de la empresa.</t>
-  </si>
-  <si>
-    <t>La dirección transmite una imagen clara de la estrategia y proyectos de la empresa.</t>
-  </si>
-  <si>
-    <t>Los cambios en las políticas y normas se comunican de inmediato a los empleados.</t>
-  </si>
-  <si>
-    <t>Se cumple la puntualidad en el pago de los salarios.</t>
-  </si>
-  <si>
-    <t>Las remuneraciones se corresponden con las exigencias y responsabilidades de los cargos.</t>
-  </si>
-  <si>
-    <t>Se premia el esfuerzo y rendimiento de los empleados mediante recompensas económicas, profesionales, etc.</t>
-  </si>
-  <si>
-    <t>Los empleados tienen posibilidad de promocionar en la empresa si realizan un buen trabajo.</t>
-  </si>
-  <si>
-    <t>Las promociones internas se realizan de manera justa, atendiendo a los mismos criterios para todos los empleados.</t>
-  </si>
-  <si>
-    <t>Los empleados tienen garantía de estabilidad laboral en corto plazo.</t>
-  </si>
-  <si>
-    <t>La temperatura del lugar trabajo es buena.</t>
-  </si>
-  <si>
-    <t>El nivel de ruido es aceptable.</t>
-  </si>
-  <si>
-    <t>Las condiciones de iluminación son buenas.</t>
-  </si>
-  <si>
-    <t>El lugar de trabajo está limpio y ordenado.</t>
-  </si>
-  <si>
-    <t>Hay espacio suficiente para que todos los empleados puedan trabajar cómodamente.</t>
-  </si>
-  <si>
-    <t>Los empleados disponen de los materiales y recursos necesarios para realizar su trabajo.</t>
-  </si>
-  <si>
-    <t>Frecuencia</t>
-  </si>
-  <si>
-    <t>Nivel Frecuencia</t>
-  </si>
-  <si>
-    <t>Error</t>
-  </si>
-  <si>
-    <t>Muy Baja</t>
-  </si>
-  <si>
-    <t>Baja</t>
-  </si>
-  <si>
-    <t>Media</t>
-  </si>
-  <si>
-    <t>Alta</t>
-  </si>
-  <si>
-    <t>Muy Alta</t>
-  </si>
-  <si>
-    <t>#</t>
-  </si>
-  <si>
-    <t>Impacto</t>
-  </si>
-  <si>
-    <t>Muy Bajo</t>
-  </si>
-  <si>
-    <t>Bajo</t>
-  </si>
-  <si>
-    <t>Medio</t>
-  </si>
-  <si>
-    <t>Alto</t>
-  </si>
-  <si>
-    <t>Muy Alto</t>
-  </si>
-  <si>
-    <t>MB</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>MA</t>
-  </si>
-  <si>
-    <t>Riesgo</t>
-  </si>
-  <si>
-    <t>Despreciable</t>
-  </si>
-  <si>
-    <t>Apreciable</t>
-  </si>
-  <si>
-    <t>Considerable</t>
-  </si>
-  <si>
-    <t>Importante</t>
-  </si>
-  <si>
-    <t>RIESGO</t>
-  </si>
-  <si>
-    <t>Implicación</t>
-  </si>
-  <si>
-    <t>Cohesión</t>
-  </si>
-  <si>
-    <t>Apoyo</t>
-  </si>
-  <si>
-    <t>Autonomía e Innovación</t>
-  </si>
-  <si>
-    <t>Jornada Laboral</t>
-  </si>
-  <si>
-    <t>Clariad</t>
-  </si>
-  <si>
-    <t>Recompensa</t>
-  </si>
-  <si>
-    <t>Lugar de Trabajo</t>
+    <t xml:space="preserve">Marque con una X la opción elegida para cada una de las preguntas:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nunca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rara vez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A veces</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normalmente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Siempre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los empleados entregan las tareas a tiempo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El personal hace un buen trabajo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los empleados muestran conductas apáticas o desinterés.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El personal llega tarde al trabajo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se convocan huelgas y paros en la organización.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los empleados faltan al trabajo sin una causa justificada.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los empleados afrontan las situaciones críticas como unidad.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los empleados se esfuerzan por integrar a los nuevos miembros en la plantilla.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los diferentes grupos de trabajo existentes colaboran entre sí.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La gente crea problemas hablando de otros a sus espaldas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La diferencia de opiniones en el equipo de trabajo provoca enfados y/o discusiones.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El ambiente de trabajo es tenso por la mala relación entre algunos empleados.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los jefes reconocen el trabajo bien hecho, y felicitan a los empleados por ello.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los jefes dialogan con sus empleados sobre lo qué hacen bien en su trabajo y los aspectos que pueden mejorar.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los empleados comentan los temas que les preocupan con sus superiores.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los jefes valoran la opinión de los empleados.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los jefes utilizan un tono autoritario para dirigirse a sus empleados.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los jefes tratan de igual forma a todos los empleados.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los empleados pueden tomar sus propias decisiones y utilizar su propia iniciativa para hacer su trabajo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los jefes se reúnen con los empleados para tomar decisiones sobre proyectos futuros.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las responsabilidades importantes se concentran en una sola persona.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se valoran  los nuevos enfoques e ideas en la realización de los trabajos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los trabajos son monótonos y repetitivos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los empleados cuentan con programas de formación para actualizar sus conocimientos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las tareas se asignan con tiempo suficiente para que se puedan realizar con calma.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los empleados tienen oportunidades para hacer pequeños descansos a lo largo del día.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los empleados tienen mucha carga de trabajo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se tienen en consideración las necesidades personales de los empleados a la hora de fijar sus horarios.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los horarios permiten la conciliación de la vida familiar y personal con la vida laboral.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ante una necesidad personal o familiar extraordinaria, se busca la mejor solución.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los empleados tienen dudas sobre cómo realizar sus tareas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se informa a los empleados de cómo contribuye su trabajo a la organización.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los jefes estimulan a los empleados para que sean precisos y ordenados.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se informa a los empleados de la situación y resultados de la empresa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La dirección transmite una imagen clara de la estrategia y proyectos de la empresa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los cambios en las políticas y normas se comunican de inmediato a los empleados.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se cumple la puntualidad en el pago de los salarios.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las remuneraciones se corresponden con las exigencias y responsabilidades de los cargos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se premia el esfuerzo y rendimiento de los empleados mediante recompensas económicas, profesionales, etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los empleados tienen posibilidad de promocionar en la empresa si realizan un buen trabajo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las promociones internas se realizan de manera justa, atendiendo a los mismos criterios para todos los empleados.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los empleados tienen garantía de estabilidad laboral en corto plazo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La temperatura del lugar trabajo es buena.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El nivel de ruido es aceptable.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las condiciones de iluminación son buenas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El lugar de trabajo está limpio y ordenado.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hay espacio suficiente para que todos los empleados puedan trabajar cómodamente.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los empleados disponen de los materiales y recursos necesarios para realizar su trabajo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frecuencia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nivel Frecuencia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muy Baja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Media</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muy Alta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impacto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muy Bajo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bajo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muy Alto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Riesgo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Despreciable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apreciable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Considerable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Importante</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RIESGO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implicación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cohesión</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apoyo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Autonomía e Innovación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jornada Laboral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clariad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recompensa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lugar de Trabajo</t>
   </si>
 </sst>
 </file>
@@ -293,7 +298,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -1152,11 +1157,10 @@
   <dxfs count="21">
     <dxf>
       <font>
-        <sz val="11"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
         <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -1166,11 +1170,10 @@
     </dxf>
     <dxf>
       <font>
-        <sz val="11"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
         <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -1180,11 +1183,10 @@
     </dxf>
     <dxf>
       <font>
-        <sz val="11"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
         <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -1194,11 +1196,10 @@
     </dxf>
     <dxf>
       <font>
-        <sz val="11"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
         <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -1208,11 +1209,10 @@
     </dxf>
     <dxf>
       <font>
-        <sz val="11"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
         <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -1222,11 +1222,10 @@
     </dxf>
     <dxf>
       <font>
-        <sz val="11"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
         <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -1236,11 +1235,10 @@
     </dxf>
     <dxf>
       <font>
-        <sz val="11"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
         <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -1250,11 +1248,10 @@
     </dxf>
     <dxf>
       <font>
-        <sz val="11"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
         <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -1264,11 +1261,10 @@
     </dxf>
     <dxf>
       <font>
-        <sz val="11"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
         <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -1278,11 +1274,10 @@
     </dxf>
     <dxf>
       <font>
-        <sz val="11"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
         <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -1292,11 +1287,10 @@
     </dxf>
     <dxf>
       <font>
-        <sz val="11"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
         <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -1306,11 +1300,10 @@
     </dxf>
     <dxf>
       <font>
-        <sz val="11"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
         <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -1320,11 +1313,10 @@
     </dxf>
     <dxf>
       <font>
-        <sz val="11"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
         <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -1334,11 +1326,10 @@
     </dxf>
     <dxf>
       <font>
-        <sz val="11"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
         <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -1348,11 +1339,10 @@
     </dxf>
     <dxf>
       <font>
-        <sz val="11"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
         <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -1362,11 +1352,10 @@
     </dxf>
     <dxf>
       <font>
-        <sz val="11"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
         <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -1376,11 +1365,10 @@
     </dxf>
     <dxf>
       <font>
-        <sz val="11"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
         <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -1390,11 +1378,10 @@
     </dxf>
     <dxf>
       <font>
-        <sz val="11"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
         <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -1404,11 +1391,10 @@
     </dxf>
     <dxf>
       <font>
-        <sz val="11"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
         <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -1418,11 +1404,10 @@
     </dxf>
     <dxf>
       <font>
-        <sz val="11"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
         <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -1432,11 +1417,10 @@
     </dxf>
     <dxf>
       <font>
-        <sz val="11"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
         <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -1513,20 +1497,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="102.570850202429"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="15.7125506072875"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.2834008097166"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="15.7125506072875"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="103.477732793522"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1598,13 +1582,13 @@
       <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C5" s="9"/>
       <c r="D5" s="10"/>
       <c r="E5" s="9"/>
       <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
+      <c r="G5" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="n">
@@ -1628,13 +1612,13 @@
       <c r="B7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="10"/>
+      <c r="C7" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
-      <c r="G7" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="G7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="n">
@@ -1645,11 +1629,11 @@
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
+      <c r="E8" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="F8" s="9"/>
-      <c r="G8" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="G8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="n">
@@ -1673,13 +1657,13 @@
       <c r="B10" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
+      <c r="G10" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="16" t="n">
@@ -1688,13 +1672,13 @@
       <c r="B11" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C11" s="9"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
+      <c r="G11" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="16" t="n">
@@ -1703,13 +1687,13 @@
       <c r="B12" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
+      <c r="G12" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="16" t="n">
@@ -1718,13 +1702,13 @@
       <c r="B13" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C13" s="9"/>
       <c r="D13" s="10"/>
       <c r="E13" s="9"/>
       <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
+      <c r="G13" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="16" t="n">
@@ -1733,13 +1717,13 @@
       <c r="B14" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C14" s="9"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="9"/>
-      <c r="G14" s="10"/>
+      <c r="G14" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="19" t="n">
@@ -1748,13 +1732,13 @@
       <c r="B15" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C15" s="9"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
-      <c r="G15" s="9"/>
+      <c r="G15" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="n">
@@ -1763,13 +1747,13 @@
       <c r="B16" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C16" s="9"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="9"/>
-      <c r="G16" s="10"/>
+      <c r="G16" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="n">
@@ -1778,13 +1762,13 @@
       <c r="B17" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C17" s="9"/>
       <c r="D17" s="10"/>
       <c r="E17" s="9"/>
       <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
+      <c r="G17" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="7" t="n">
@@ -1793,13 +1777,13 @@
       <c r="B18" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
+      <c r="G18" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="n">
@@ -1808,13 +1792,13 @@
       <c r="B19" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C19" s="9"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
+      <c r="G19" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="n">
@@ -1823,13 +1807,13 @@
       <c r="B20" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C20" s="9"/>
       <c r="D20" s="9"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
+      <c r="G20" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="23" t="n">
@@ -1838,13 +1822,13 @@
       <c r="B21" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C21" s="9"/>
       <c r="D21" s="10"/>
       <c r="E21" s="9"/>
       <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
+      <c r="G21" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="24" t="n">
@@ -1853,13 +1837,13 @@
       <c r="B22" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C22" s="9"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="9"/>
-      <c r="G22" s="10"/>
+      <c r="G22" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="24" t="n">
@@ -1868,13 +1852,13 @@
       <c r="B23" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C23" s="9"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
-      <c r="G23" s="9"/>
+      <c r="G23" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="24" t="n">
@@ -1883,13 +1867,13 @@
       <c r="B24" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C24" s="9"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
       <c r="F24" s="9"/>
-      <c r="G24" s="10"/>
+      <c r="G24" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="24" t="n">
@@ -1898,13 +1882,13 @@
       <c r="B25" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C25" s="9"/>
       <c r="D25" s="10"/>
       <c r="E25" s="9"/>
       <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
+      <c r="G25" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="24" t="n">
@@ -1913,13 +1897,13 @@
       <c r="B26" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C26" s="9"/>
       <c r="D26" s="9"/>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
+      <c r="G26" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="7" t="n">
@@ -1928,13 +1912,13 @@
       <c r="B27" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C27" s="9"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
+      <c r="G27" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="19" t="n">
@@ -1943,13 +1927,13 @@
       <c r="B28" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C28" s="9"/>
       <c r="D28" s="9"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
+      <c r="G28" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="7" t="n">
@@ -1958,13 +1942,13 @@
       <c r="B29" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C29" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C29" s="9"/>
       <c r="D29" s="10"/>
       <c r="E29" s="9"/>
       <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
+      <c r="G29" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="26" t="n">
@@ -1973,13 +1957,13 @@
       <c r="B30" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C30" s="9"/>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
       <c r="F30" s="9"/>
-      <c r="G30" s="10"/>
+      <c r="G30" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="26" t="n">
@@ -1988,13 +1972,13 @@
       <c r="B31" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C31" s="9"/>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
-      <c r="G31" s="9"/>
+      <c r="G31" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="7" t="n">
@@ -2003,13 +1987,13 @@
       <c r="B32" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C32" s="9"/>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
       <c r="F32" s="9"/>
-      <c r="G32" s="10"/>
+      <c r="G32" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="28" t="n">
@@ -2018,13 +2002,13 @@
       <c r="B33" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C33" s="9"/>
       <c r="D33" s="10"/>
       <c r="E33" s="9"/>
       <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
+      <c r="G33" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="16" t="n">
@@ -2033,13 +2017,13 @@
       <c r="B34" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C34" s="9"/>
       <c r="D34" s="9"/>
       <c r="E34" s="10"/>
       <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
+      <c r="G34" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="14" t="n">
@@ -2048,13 +2032,13 @@
       <c r="B35" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C35" s="9"/>
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
       <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
+      <c r="G35" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="14" t="n">
@@ -2063,13 +2047,13 @@
       <c r="B36" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C36" s="9"/>
       <c r="D36" s="9"/>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
+      <c r="G36" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="14" t="n">
@@ -2078,13 +2062,13 @@
       <c r="B37" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C37" s="9"/>
       <c r="D37" s="10"/>
       <c r="E37" s="9"/>
       <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
+      <c r="G37" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="14" t="n">
@@ -2093,13 +2077,13 @@
       <c r="B38" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C38" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C38" s="9"/>
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
       <c r="F38" s="9"/>
-      <c r="G38" s="10"/>
+      <c r="G38" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="30" t="n">
@@ -2108,13 +2092,13 @@
       <c r="B39" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C39" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C39" s="9"/>
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
-      <c r="G39" s="9"/>
+      <c r="G39" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="31" t="n">
@@ -2123,13 +2107,13 @@
       <c r="B40" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="C40" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C40" s="9"/>
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
       <c r="F40" s="9"/>
-      <c r="G40" s="10"/>
+      <c r="G40" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="31" t="n">
@@ -2138,13 +2122,13 @@
       <c r="B41" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="C41" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C41" s="9"/>
       <c r="D41" s="10"/>
       <c r="E41" s="9"/>
       <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
+      <c r="G41" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="31" t="n">
@@ -2153,13 +2137,13 @@
       <c r="B42" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="C42" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C42" s="9"/>
       <c r="D42" s="9"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
+      <c r="G42" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="31" t="n">
@@ -2168,13 +2152,13 @@
       <c r="B43" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="C43" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C43" s="9"/>
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
-      <c r="G43" s="10"/>
+      <c r="G43" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="31" t="n">
@@ -2183,13 +2167,13 @@
       <c r="B44" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="C44" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C44" s="9"/>
       <c r="D44" s="9"/>
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
-      <c r="G44" s="10"/>
+      <c r="G44" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="33" t="n">
@@ -2198,13 +2182,13 @@
       <c r="B45" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="C45" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C45" s="9"/>
       <c r="D45" s="10"/>
       <c r="E45" s="9"/>
       <c r="F45" s="10"/>
-      <c r="G45" s="10"/>
+      <c r="G45" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="35" t="n">
@@ -2213,13 +2197,13 @@
       <c r="B46" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="C46" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C46" s="9"/>
       <c r="D46" s="10"/>
       <c r="E46" s="10"/>
       <c r="F46" s="9"/>
-      <c r="G46" s="10"/>
+      <c r="G46" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="35" t="n">
@@ -2228,13 +2212,13 @@
       <c r="B47" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="C47" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C47" s="9"/>
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
       <c r="F47" s="10"/>
-      <c r="G47" s="9"/>
+      <c r="G47" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="37" t="n">
@@ -2243,13 +2227,13 @@
       <c r="B48" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="C48" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C48" s="9"/>
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
       <c r="F48" s="9"/>
-      <c r="G48" s="10"/>
+      <c r="G48" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="37" t="n">
@@ -2258,13 +2242,13 @@
       <c r="B49" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="C49" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C49" s="9"/>
       <c r="D49" s="10"/>
       <c r="E49" s="9"/>
       <c r="F49" s="10"/>
-      <c r="G49" s="10"/>
+      <c r="G49" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="37" t="n">
@@ -2273,14 +2257,18 @@
       <c r="B50" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="C50" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C50" s="9"/>
       <c r="D50" s="9"/>
       <c r="E50" s="10"/>
       <c r="F50" s="10"/>
-      <c r="G50" s="10"/>
-    </row>
+      <c r="G50" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
@@ -3264,31 +3252,31 @@
   </sheetPr>
   <dimension ref="A1:Q49"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q11" activeCellId="0" sqref="Q11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N16" activeCellId="0" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.9959514170041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.2834008097166"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="11.8542510121458"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="14.8542510121458"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.5668016194332"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.5748987854251"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.7165991902834"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.8542510121457"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.4251012145749"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.5668016194332"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="17" min="16" style="0" width="12.2834008097166"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.8542510121458"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.5668016194332"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.1417004048583"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="8.2834008097166"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.1052631578947"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3562753036437"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="11.9959514170041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.7125506072875"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.9271255060729"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="17" min="16" style="0" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.9959514170041"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.6032388663968"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="8.35627530364373"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3339,11 +3327,11 @@
       </c>
       <c r="G2" s="45" t="n">
         <f aca="false">SUM(B2:F7)</f>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H2" s="46" t="str">
         <f aca="false">IF(AND(G2&gt;5,G2&lt;11),L3,IF(AND(G2&gt;10,G2&lt;16),M3,IF(AND(G2&gt;15,G2&lt;21),N3,IF(AND(G2&lt;26,G2&gt;20),O3,IF(AND(G2&gt;25,G2&lt;31),P3,Q3)))))</f>
-        <v>Alta</v>
+        <v>Media</v>
       </c>
       <c r="Q2" s="47" t="s">
         <v>58</v>
@@ -3403,7 +3391,7 @@
       </c>
       <c r="B4" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!C5=A1,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!D5=A1,2,0)</f>
@@ -3419,7 +3407,7 @@
       </c>
       <c r="F4" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!G5=A1,5,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G4" s="45"/>
       <c r="H4" s="46"/>
@@ -3493,7 +3481,7 @@
       </c>
       <c r="B6" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!C7=A1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!D7=A1,2,0)</f>
@@ -3509,7 +3497,7 @@
       </c>
       <c r="F6" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!G7=A1,5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G6" s="45"/>
       <c r="H6" s="46"/>
@@ -3546,7 +3534,7 @@
       </c>
       <c r="D7" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!E8=A1,3,0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E7" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!F8=A1,2,0)</f>
@@ -3554,7 +3542,7 @@
       </c>
       <c r="F7" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!G8=A1,5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G7" s="45"/>
       <c r="H7" s="46"/>
@@ -3585,11 +3573,11 @@
       </c>
       <c r="G8" s="45" t="n">
         <f aca="false">SUM(B8:F13)</f>
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H8" s="46" t="str">
         <f aca="false">IF(AND(G8&gt;5,G8&lt;11),L3,IF(AND(G8&gt;10,G8&lt;16),M3,IF(AND(G8&gt;15,G8&lt;21),N3,IF(AND(G8&lt;26,G8&gt;20),O3,IF(AND(G8&gt;25,G8&lt;31),P3,Q3)))))</f>
-        <v>Media</v>
+        <v>Alta</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3598,7 +3586,7 @@
       </c>
       <c r="B9" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!C10=A1,5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C9" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!D10=A1,4,0)</f>
@@ -3614,7 +3602,7 @@
       </c>
       <c r="F9" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!G10=A1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="45"/>
       <c r="H9" s="46"/>
@@ -3625,7 +3613,7 @@
       </c>
       <c r="B10" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!C11=A1,5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C10" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!D11=A1,4,0)</f>
@@ -3641,7 +3629,7 @@
       </c>
       <c r="F10" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!G11=A1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="45"/>
       <c r="H10" s="46"/>
@@ -3654,7 +3642,7 @@
       </c>
       <c r="B11" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!C12=A1,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!D12=A1,2,0)</f>
@@ -3670,7 +3658,7 @@
       </c>
       <c r="F11" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!G12=A1,5,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G11" s="45"/>
       <c r="H11" s="46"/>
@@ -3692,7 +3680,7 @@
       </c>
       <c r="Q11" s="63" t="n">
         <f aca="false">(SUM(N12:N19))/8</f>
-        <v>7.625</v>
+        <v>3.625</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3701,7 +3689,7 @@
       </c>
       <c r="B12" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!C13=A1,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!D13=A1,2,0)</f>
@@ -3717,7 +3705,7 @@
       </c>
       <c r="F12" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!G13=A1,5,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G12" s="45"/>
       <c r="H12" s="46"/>
@@ -3730,7 +3718,7 @@
       </c>
       <c r="L12" s="66" t="str">
         <f aca="false">IF(H2=L3,L5,IF(H2=M3,M5,IF(H2=N3,N5,IF(H2=O3,O5,IF(H2=P3,P5,Q3)))))</f>
-        <v>A</v>
+        <v>M</v>
       </c>
       <c r="M12" s="66" t="str">
         <f aca="false">IF(L12=L5,M5,IF(L12=M5,N5,IF(L12=N5,O5,IF(L12=O5,O5,IF(L12=P5,P5,Q3)))))</f>
@@ -3749,7 +3737,7 @@
       </c>
       <c r="B13" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!C14=A1,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!D14=A1,2,0)</f>
@@ -3765,7 +3753,7 @@
       </c>
       <c r="F13" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!G14=A1,5,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G13" s="45"/>
       <c r="H13" s="46"/>
@@ -3778,15 +3766,15 @@
       </c>
       <c r="L13" s="66" t="str">
         <f aca="false">IF(H8=L3,L5,IF(H8=M3,M5,IF(H8=N3,N5,IF(H8=O3,O5,IF(H8=P3,P5,Q3)))))</f>
-        <v>M</v>
+        <v>A</v>
       </c>
       <c r="M13" s="66" t="str">
         <f aca="false">IF(L13=L5,M5,IF(L13=M5,N5,IF(L13=N5,N5,IF(L13=O5,O5,IF(L13=P5,O5,Q3)))))</f>
-        <v>M</v>
+        <v>A</v>
       </c>
       <c r="N13" s="47" t="n">
         <f aca="false">IF(M13=L5,0,IF(M13=M5,2,IF(M13=N5,5,IF(M13=O5,8,IF(M13=P5,10,Q3)))))</f>
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3795,7 +3783,7 @@
       </c>
       <c r="B14" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!C15=A1,5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C14" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!D15=A1,4,0)</f>
@@ -3811,15 +3799,15 @@
       </c>
       <c r="F14" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!G15=A1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="45" t="n">
         <f aca="false">SUM(B14:F19)</f>
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="H14" s="46" t="str">
         <f aca="false">IF(AND(G14&gt;5,G14&lt;11),L3,IF(AND(G14&gt;10,G14&lt;16),M3,IF(AND(G14&gt;15,G14&lt;21),N3,IF(AND(G14&lt;26,G14&gt;20),O3,IF(AND(G14&gt;25,G14&lt;31),P3,Q3)))))</f>
-        <v>Muy Alta</v>
+        <v>Muy Baja</v>
       </c>
       <c r="J14" s="64" t="s">
         <v>84</v>
@@ -3830,15 +3818,15 @@
       </c>
       <c r="L14" s="66" t="str">
         <f aca="false">IF(H14=L3,L5,IF(H14=M3,M5,IF(H14=N3,N5,IF(H14=O3,O5,IF(H14=P3,P5,Q3)))))</f>
-        <v>MA</v>
+        <v>MB</v>
       </c>
       <c r="M14" s="66" t="str">
         <f aca="false">IF(L14=L5,M5,IF(L14=M5,N5,IF(L14=N5,N5,IF(L14=O5,O5,IF(L14=P5,O5,Q3)))))</f>
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="N14" s="47" t="n">
         <f aca="false">IF(M14=L5,0,IF(M14=M5,2,IF(M14=N5,5,IF(M14=O5,8,IF(M14=P5,10,Q3)))))</f>
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3847,7 +3835,7 @@
       </c>
       <c r="B15" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!C16=A1,5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C15" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!D16=A1,4,0)</f>
@@ -3863,7 +3851,7 @@
       </c>
       <c r="F15" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!G16=A1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" s="45"/>
       <c r="H15" s="46"/>
@@ -3876,15 +3864,15 @@
       </c>
       <c r="L15" s="66" t="str">
         <f aca="false">IF(H20=L3,L5,IF(H20=M3,M5,IF(H20=N3,N5,IF(H20=O3,O5,IF(H20=P3,P5,Q3)))))</f>
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="M15" s="66" t="str">
         <f aca="false">IF(L15=L5,M5,IF(L15=M5,N5,IF(L15=N5,N5,IF(L15=O5,O5,IF(L15=P5,O5,Q3)))))</f>
-        <v>A</v>
+        <v>M</v>
       </c>
       <c r="N15" s="47" t="n">
         <f aca="false">IF(M15=L5,0,IF(M15=M5,2,IF(M15=N5,5,IF(M15=O5,8,IF(M15=P5,10,Q3)))))</f>
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3893,7 +3881,7 @@
       </c>
       <c r="B16" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!C17=A1,5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C16" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!D17=A1,4,0)</f>
@@ -3909,7 +3897,7 @@
       </c>
       <c r="F16" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!G17=A1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="45"/>
       <c r="H16" s="46"/>
@@ -3922,15 +3910,15 @@
       </c>
       <c r="L16" s="66" t="str">
         <f aca="false">IF(H26=L3,L5,IF(H26=M3,M5,IF(H26=N3,N5,IF(H26=O3,O5,IF(H26=P3,P5,Q3)))))</f>
-        <v>MA</v>
+        <v>MB</v>
       </c>
       <c r="M16" s="66" t="str">
         <f aca="false">IF(L16=L5,M5,IF(L16=M5,N5,IF(L16=N5,N5,IF(L16=O5,O5,IF(L16=P5,O5,Q3)))))</f>
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="N16" s="47" t="n">
         <f aca="false">IF(M16=L5,0,IF(M16=M5,2,IF(M16=N5,5,IF(M16=O5,8,IF(M16=P5,10,Q3)))))</f>
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3939,7 +3927,7 @@
       </c>
       <c r="B17" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!C18=A1,5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C17" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!D18=A1,4,0)</f>
@@ -3955,7 +3943,7 @@
       </c>
       <c r="F17" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!G18=A1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" s="45"/>
       <c r="H17" s="46"/>
@@ -3968,15 +3956,15 @@
       </c>
       <c r="L17" s="66" t="str">
         <f aca="false">IF(H32=L3,L5,IF(H32=M3,M5,IF(H32=N3,N5,IF(H32=O3,O5,IF(H32=P3,P5,Q3)))))</f>
-        <v>MA</v>
+        <v>MB</v>
       </c>
       <c r="M17" s="66" t="str">
         <f aca="false">IF(L17=L5,M5,IF(L17=M5,M5,IF(L17=N5,N5,IF(L17=O5,N5,IF(L17=P5,O5,Q3)))))</f>
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="N17" s="47" t="n">
         <f aca="false">IF(M17=L5,0,IF(M17=M5,2,IF(M17=N5,5,IF(M17=O5,8,IF(M17=P5,10,Q3)))))</f>
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3985,7 +3973,7 @@
       </c>
       <c r="B18" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!C19=A1,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!D19=A1,2,0)</f>
@@ -4001,7 +3989,7 @@
       </c>
       <c r="F18" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!G19=A1,5,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G18" s="45"/>
       <c r="H18" s="46"/>
@@ -4014,15 +4002,15 @@
       </c>
       <c r="L18" s="66" t="str">
         <f aca="false">IF(H38=L3,L5,IF(H38=M3,M5,IF(H38=N3,N5,IF(H38=O3,O5,IF(H38=P3,P5,Q3)))))</f>
-        <v>MA</v>
+        <v>MB</v>
       </c>
       <c r="M18" s="66" t="str">
         <f aca="false">IF(L18=L5,M5,IF(L18=M5,N5,IF(L18=N5,N5,IF(L18=O5,O5,IF(L18=P5,O5,Q3)))))</f>
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="N18" s="47" t="n">
         <f aca="false">IF(M18=L5,0,IF(M18=M5,2,IF(M18=N5,5,IF(M18=O5,8,IF(M18=P5,10,Q3)))))</f>
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4031,7 +4019,7 @@
       </c>
       <c r="B19" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!C20=A1,5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C19" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!D20=A1,4,0)</f>
@@ -4047,7 +4035,7 @@
       </c>
       <c r="F19" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!G20=A1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" s="45"/>
       <c r="H19" s="46"/>
@@ -4060,15 +4048,15 @@
       </c>
       <c r="L19" s="66" t="str">
         <f aca="false">IF(H44=L3,L5,IF(H44=M3,M5,IF(H44=N3,N5,IF(H44=O3,O5,IF(H44=P3,P5,Q3)))))</f>
-        <v>MA</v>
+        <v>#</v>
       </c>
       <c r="M19" s="66" t="str">
         <f aca="false">IF(L19=L5,M5,IF(L19=M5,M5,IF(L19=N5,N5,IF(L19=O5,N5,IF(L19=P5,O5,Q3)))))</f>
-        <v>A</v>
-      </c>
-      <c r="N19" s="47" t="n">
+        <v>#</v>
+      </c>
+      <c r="N19" s="47" t="str">
         <f aca="false">IF(M19=L5,0,IF(M19=M5,2,IF(M19=N5,5,IF(M19=O5,8,IF(M19=P5,10,Q3)))))</f>
-        <v>8</v>
+        <v>#</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4077,7 +4065,7 @@
       </c>
       <c r="B20" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!C21=A1,5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C20" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!D21=A1,4,0)</f>
@@ -4093,15 +4081,15 @@
       </c>
       <c r="F20" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!G21=A1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" s="45" t="n">
         <f aca="false">SUM(B20:F25)</f>
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H20" s="46" t="str">
         <f aca="false">IF(AND(G20&gt;5,G20&lt;11),L3,IF(AND(G20&gt;10,G20&lt;16),M3,IF(AND(G20&gt;15,G20&lt;21),N3,IF(AND(G20&lt;26,G20&gt;20),O3,IF(AND(G20&gt;25,G20&lt;31),P3,Q3)))))</f>
-        <v>Alta</v>
+        <v>Baja</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4110,7 +4098,7 @@
       </c>
       <c r="B21" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!C22=A1,5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C21" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!D22=A1,4,0)</f>
@@ -4126,7 +4114,7 @@
       </c>
       <c r="F21" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!G22=A1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21" s="45"/>
       <c r="H21" s="46"/>
@@ -4137,7 +4125,7 @@
       </c>
       <c r="B22" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!C23=A1,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!D23=A1,2,0)</f>
@@ -4153,7 +4141,7 @@
       </c>
       <c r="F22" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!G23=A1,5,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G22" s="45"/>
       <c r="H22" s="46"/>
@@ -4164,7 +4152,7 @@
       </c>
       <c r="B23" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!C24=A1,5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C23" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!D24=A1,4,0)</f>
@@ -4180,7 +4168,7 @@
       </c>
       <c r="F23" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!G24=A1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" s="45"/>
       <c r="H23" s="46"/>
@@ -4191,7 +4179,7 @@
       </c>
       <c r="B24" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!C25=A1,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!D25=A1,2,0)</f>
@@ -4207,7 +4195,7 @@
       </c>
       <c r="F24" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!G25=A1,5,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G24" s="45"/>
       <c r="H24" s="46"/>
@@ -4218,7 +4206,7 @@
       </c>
       <c r="B25" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!C26=A1,5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C25" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!D26=A1,4,0)</f>
@@ -4234,7 +4222,7 @@
       </c>
       <c r="F25" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!G26=A1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" s="45"/>
       <c r="H25" s="46"/>
@@ -4245,7 +4233,7 @@
       </c>
       <c r="B26" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!C27=A1,5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C26" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!D27=A1,4,0)</f>
@@ -4261,15 +4249,15 @@
       </c>
       <c r="F26" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!G27=A1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26" s="45" t="n">
         <f aca="false">SUM(B26:F31)</f>
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="H26" s="46" t="str">
         <f aca="false">IF(AND(G26&gt;5,G26&lt;11),L3,IF(AND(G26&gt;10,G26&lt;16),M3,IF(AND(G26&gt;15,G26&lt;21),N3,IF(AND(G26&lt;26,G26&gt;20),O3,IF(AND(G26&gt;25,G26&lt;31),P3,Q3)))))</f>
-        <v>Muy Alta</v>
+        <v>Muy Baja</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4278,7 +4266,7 @@
       </c>
       <c r="B27" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!C28=A1,5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C27" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!D28=A1,4,0)</f>
@@ -4294,7 +4282,7 @@
       </c>
       <c r="F27" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!G28=A1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27" s="45"/>
       <c r="H27" s="46"/>
@@ -4305,7 +4293,7 @@
       </c>
       <c r="B28" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!C29=A1,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C28" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!D29=A1,2,0)</f>
@@ -4321,7 +4309,7 @@
       </c>
       <c r="F28" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!G29=A1,5,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G28" s="45"/>
       <c r="H28" s="46"/>
@@ -4332,7 +4320,7 @@
       </c>
       <c r="B29" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!C30=A1,5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C29" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!D30=A1,4,0)</f>
@@ -4348,7 +4336,7 @@
       </c>
       <c r="F29" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!G30=A1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29" s="45"/>
       <c r="H29" s="46"/>
@@ -4359,7 +4347,7 @@
       </c>
       <c r="B30" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!C31=A1,5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C30" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!D31=A1,4,0)</f>
@@ -4375,7 +4363,7 @@
       </c>
       <c r="F30" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!G31=A1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30" s="45"/>
       <c r="H30" s="46"/>
@@ -4386,7 +4374,7 @@
       </c>
       <c r="B31" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!C32=A1,5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C31" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!D32=A1,4,0)</f>
@@ -4402,7 +4390,7 @@
       </c>
       <c r="F31" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!G32=A1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31" s="45"/>
       <c r="H31" s="46"/>
@@ -4413,7 +4401,7 @@
       </c>
       <c r="B32" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!C33=A1,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C32" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!D33=A1,2,0)</f>
@@ -4429,15 +4417,15 @@
       </c>
       <c r="F32" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!G33=A1,5,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G32" s="45" t="n">
         <f aca="false">SUM(B32:F37)</f>
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="H32" s="46" t="str">
         <f aca="false">IF(AND(G32&gt;5,G32&lt;11),L3,IF(AND(G32&gt;10,G32&lt;16),M3,IF(AND(G32&gt;15,G32&lt;21),N3,IF(AND(G32&lt;26,G32&gt;20),O3,IF(AND(G32&gt;25,G32&lt;31),P3,Q3)))))</f>
-        <v>Muy Alta</v>
+        <v>Muy Baja</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4446,7 +4434,7 @@
       </c>
       <c r="B33" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!C34=A1,5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C33" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!D34=A1,4,0)</f>
@@ -4462,7 +4450,7 @@
       </c>
       <c r="F33" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!G34=A1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33" s="45"/>
       <c r="H33" s="46"/>
@@ -4473,7 +4461,7 @@
       </c>
       <c r="B34" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!C35=A1,5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C34" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!D35=A1,4,0)</f>
@@ -4489,7 +4477,7 @@
       </c>
       <c r="F34" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!G35=A1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G34" s="45"/>
       <c r="H34" s="46"/>
@@ -4500,7 +4488,7 @@
       </c>
       <c r="B35" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!C36=A1,5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C35" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!D36=A1,4,0)</f>
@@ -4516,7 +4504,7 @@
       </c>
       <c r="F35" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!G36=A1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G35" s="45"/>
       <c r="H35" s="46"/>
@@ -4527,7 +4515,7 @@
       </c>
       <c r="B36" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!C37=A1,5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C36" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!D37=A1,4,0)</f>
@@ -4543,7 +4531,7 @@
       </c>
       <c r="F36" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!G37=A1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G36" s="45"/>
       <c r="H36" s="46"/>
@@ -4554,7 +4542,7 @@
       </c>
       <c r="B37" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!C38=A1,5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C37" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!D38=A1,4,0)</f>
@@ -4570,7 +4558,7 @@
       </c>
       <c r="F37" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!G38=A1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G37" s="45"/>
       <c r="H37" s="46"/>
@@ -4581,7 +4569,7 @@
       </c>
       <c r="B38" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!C39=A1,5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C38" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!D39=A1,4,0)</f>
@@ -4597,15 +4585,15 @@
       </c>
       <c r="F38" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!G39=A1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G38" s="45" t="n">
         <f aca="false">SUM(B38:F43)</f>
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="H38" s="46" t="str">
         <f aca="false">IF(AND(G38&gt;5,G38&lt;11),L3,IF(AND(G38&gt;10,G38&lt;16),M3,IF(AND(G38&gt;15,G38&lt;21),N3,IF(AND(G38&lt;26,G38&gt;20),O3,IF(AND(G38&gt;25,G38&lt;31),P3,Q3)))))</f>
-        <v>Muy Alta</v>
+        <v>Muy Baja</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4614,7 +4602,7 @@
       </c>
       <c r="B39" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!C40=A1,5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C39" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!D40=A1,4,0)</f>
@@ -4630,7 +4618,7 @@
       </c>
       <c r="F39" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!G40=A1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G39" s="45"/>
       <c r="H39" s="46"/>
@@ -4641,7 +4629,7 @@
       </c>
       <c r="B40" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!C41=A1,5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C40" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!D41=A1,4,0)</f>
@@ -4657,7 +4645,7 @@
       </c>
       <c r="F40" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!G41=A1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G40" s="45"/>
       <c r="H40" s="46"/>
@@ -4668,7 +4656,7 @@
       </c>
       <c r="B41" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!C42=A1,5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C41" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!D42=A1,4,0)</f>
@@ -4684,7 +4672,7 @@
       </c>
       <c r="F41" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!G42=A1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G41" s="45"/>
       <c r="H41" s="46"/>
@@ -4695,7 +4683,7 @@
       </c>
       <c r="B42" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!C43=A1,5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C42" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!D43=A1,4,0)</f>
@@ -4711,7 +4699,7 @@
       </c>
       <c r="F42" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!G43=A1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G42" s="45"/>
       <c r="H42" s="46"/>
@@ -4722,7 +4710,7 @@
       </c>
       <c r="B43" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!C44=A1,5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C43" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!D44=A1,4,0)</f>
@@ -4738,7 +4726,7 @@
       </c>
       <c r="F43" s="44" t="n">
         <f aca="false">IF(+CUESTIONARIO!G44=A1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G43" s="45"/>
       <c r="H43" s="46"/>
@@ -4749,7 +4737,7 @@
       </c>
       <c r="B44" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!C45=A1,5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C44" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!D45=A1,4,0)</f>
@@ -4769,11 +4757,11 @@
       </c>
       <c r="G44" s="45" t="n">
         <f aca="false">SUM(B44:F49)</f>
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="H44" s="46" t="str">
         <f aca="false">IF(AND(G44&gt;5,G44&lt;11),L3,IF(AND(G44&gt;10,G44&lt;16),M3,IF(AND(G44&gt;15,G44&lt;21),N3,IF(AND(G44&lt;26,G44&gt;20),O3,IF(AND(G44&gt;25,G44&lt;31),P3,Q3)))))</f>
-        <v>Muy Alta</v>
+        <v>#</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4782,7 +4770,7 @@
       </c>
       <c r="B45" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!C46=A1,5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C45" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!D46=A1,4,0)</f>
@@ -4798,7 +4786,7 @@
       </c>
       <c r="F45" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!G46=A1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G45" s="45"/>
       <c r="H45" s="46"/>
@@ -4809,7 +4797,7 @@
       </c>
       <c r="B46" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!C47=A1,5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C46" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!D47=A1,4,0)</f>
@@ -4825,7 +4813,7 @@
       </c>
       <c r="F46" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!G47=A1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G46" s="45"/>
       <c r="H46" s="46"/>
@@ -4836,7 +4824,7 @@
       </c>
       <c r="B47" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!C48=A1,5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C47" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!D48=A1,4,0)</f>
@@ -4852,7 +4840,7 @@
       </c>
       <c r="F47" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!G48=A1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G47" s="45"/>
       <c r="H47" s="46"/>
@@ -4863,7 +4851,7 @@
       </c>
       <c r="B48" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!C49=A1,5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C48" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!D49=A1,4,0)</f>
@@ -4879,7 +4867,7 @@
       </c>
       <c r="F48" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!G49=A1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G48" s="45"/>
       <c r="H48" s="46"/>
@@ -4890,7 +4878,7 @@
       </c>
       <c r="B49" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!C50=A1,5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C49" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!D50=A1,4,0)</f>
@@ -4906,7 +4894,7 @@
       </c>
       <c r="F49" s="58" t="n">
         <f aca="false">IF(+CUESTIONARIO!G50=A1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G49" s="45"/>
       <c r="H49" s="46"/>

</xml_diff>

<commit_message>
commit final Luis :(
</commit_message>
<xml_diff>
--- a/sensors/social/sensorSocial.xlsx
+++ b/sensors/social/sensorSocial.xlsx
@@ -1154,279 +1154,42 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="12">
     <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6699"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
     <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
     <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
     <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB4C7E7"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
     <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDBDBDB"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
     <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBDD7EE"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
     <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
     <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
     <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6699"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
     <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBDD7EE"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
     <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
     <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBDD7EE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBDD7EE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6699"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
   </dxfs>
   <colors>
@@ -1500,16 +1263,16 @@
   <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G51" activeCellId="0" sqref="G51"/>
+      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="104.331983805668"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="105.2995951417"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="15.9595141700405"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3251,28 +3014,28 @@
   <dimension ref="A1:Q49"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N16" activeCellId="0" sqref="N16"/>
+      <selection pane="topLeft" activeCell="Q13" activeCellId="0" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.3198380566802"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="12.1052631578947"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.1052631578947"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.8178137651822"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.9230769230769"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="24.3157894736842"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.9271255060729"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="17" min="16" style="0" width="12.5344129554656"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.1052631578947"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="17" min="16" style="0" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.2105263157895"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="0" width="8.35627530364373"/>
     <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.57085020242915"/>
   </cols>
@@ -3634,7 +3397,7 @@
       <c r="N10" s="59"/>
       <c r="Q10" s="60"/>
     </row>
-    <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="57" t="n">
         <v>10</v>
       </c>
@@ -3677,11 +3440,10 @@
         <v>81</v>
       </c>
       <c r="Q11" s="63" t="n">
-        <f aca="false">(SUM(N12:N19))/8</f>
-        <v>5.75</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8.3</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="57" t="n">
         <v>11</v>
       </c>
@@ -3729,7 +3491,7 @@
       <c r="P12" s="62"/>
       <c r="Q12" s="63"/>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="57" t="n">
         <v>12</v>
       </c>
@@ -4928,66 +4690,66 @@
     <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>$O$5</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>$P$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M12:M19">
-    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>$M$5</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="7" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="cellIs" priority="7" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>$N$5</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="8" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="cellIs" priority="8" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>$O$5</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="9" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="cellIs" priority="9" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>$P$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L13">
-    <cfRule type="cellIs" priority="10" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="cellIs" priority="10" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>$M$5</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="11" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="11" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>$N$5</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="12" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="cellIs" priority="12" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>$O$5</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="13" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="cellIs" priority="13" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>$P$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L17">
-    <cfRule type="cellIs" priority="14" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="cellIs" priority="14" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>$M$5</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="15" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+    <cfRule type="cellIs" priority="15" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>$N$5</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="16" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+    <cfRule type="cellIs" priority="16" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>$O$5</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="17" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
+    <cfRule type="cellIs" priority="17" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>$P$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L18">
-    <cfRule type="cellIs" priority="18" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
+    <cfRule type="cellIs" priority="18" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>$P$5</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="19" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
+    <cfRule type="cellIs" priority="19" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>$O$5</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="20" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18">
+    <cfRule type="cellIs" priority="20" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>$N$5</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="21" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19">
+    <cfRule type="cellIs" priority="21" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>$M$5</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="22" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20">
+    <cfRule type="cellIs" priority="22" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>$L$5</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>